<commit_message>
Add Light tracking experiment results
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiba\Documents\ENSAM\3A - Bristol\Robotic Systems\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Famous\Documents\Robotics_Masters\NOTES\Robotic_Systems\RS_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CCD254-27E4-4493-81EE-F2D7ADC211A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15146078-86CD-443E-AC5C-C8558B03E0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{8216E25C-A24B-4AD6-9FC1-220EFE9DF34B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{8216E25C-A24B-4AD6-9FC1-220EFE9DF34B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Angle</t>
   </si>
@@ -115,6 +115,54 @@
   </si>
   <si>
     <t>Distance Variation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light_Tracking </t>
+  </si>
+  <si>
+    <t>Distance from Source</t>
+  </si>
+  <si>
+    <t>IR Height</t>
+  </si>
+  <si>
+    <t>Angle - Alpha(degrees)</t>
+  </si>
+  <si>
+    <t>Tine Elapsed(s)</t>
+  </si>
+  <si>
+    <t>Average Time</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
   </si>
 </sst>
 </file>
@@ -287,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -304,6 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -324,7 +373,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -361,7 +410,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -935,7 +984,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="41510752"/>
@@ -997,7 +1046,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="41521984"/>
@@ -1039,7 +1088,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1076,7 +1125,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1090,7 +1139,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1127,7 +1176,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1296,7 +1345,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2066579968"/>
@@ -1358,7 +1407,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2066583712"/>
@@ -1406,7 +1455,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1420,7 +1469,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1457,7 +1506,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1626,7 +1675,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2061869728"/>
@@ -1688,7 +1737,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2061867648"/>
@@ -1736,7 +1785,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3528,8 +3577,27 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A710DFCB-D8FF-48C7-BEEC-661FB7BC206B}" name="Table1" displayName="Table1" ref="A44:J52" totalsRowShown="0">
+  <autoFilter ref="A44:J52" xr:uid="{A710DFCB-D8FF-48C7-BEEC-661FB7BC206B}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{46E0E1EC-FF77-4040-896D-EA505643B8F5}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{5CD028DF-B80B-413D-A9E0-657F3C32B814}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{8EBB361E-57F2-47A1-A6AA-246022CBEBFB}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{AB38F2E4-6F7A-418B-8E39-AA0802173448}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{53636D60-7758-44C9-B254-05EFDF3D7E13}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{33418470-90A6-4352-B02F-88CF920DEB1E}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{625951A2-724F-471A-8104-1D82661E42DA}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{553EFC4E-9436-498D-B66E-A2226A9890FB}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{ACE78536-4851-4854-94EA-8673FD897527}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{FE7D2C8B-A2DE-44F8-8460-63D359C45E4D}" name="Column10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3825,20 +3893,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5075D8FF-A720-421E-AF80-CE3859848E9E}">
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -3885,7 +3964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>-30</v>
       </c>
@@ -3934,7 +4013,7 @@
         <v>4.2451332919787896</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>-15</v>
       </c>
@@ -3983,7 +4062,7 @@
         <v>0.81242025249661609</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -4032,7 +4111,7 @@
         <v>0.70731416876331077</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>15</v>
       </c>
@@ -4081,7 +4160,7 @@
         <v>0.75611654010623419</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>30</v>
       </c>
@@ -4130,12 +4209,12 @@
         <v>1.6999071870088802</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>0</v>
       </c>
@@ -4182,7 +4261,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -4231,7 +4310,7 @@
         <v>0.70731416876331077</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -4280,7 +4359,7 @@
         <v>0.68702983923553052</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -4329,7 +4408,7 @@
         <v>0.49311819633385318</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -4378,7 +4457,7 @@
         <v>0.37525694900664713</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>0</v>
       </c>
@@ -4427,27 +4506,27 @@
         <v>0.42740171059814708</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>22</v>
       </c>
@@ -4509,7 +4588,7 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
         <v>24</v>
       </c>
@@ -4571,7 +4650,7 @@
         <v>484.78</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>23</v>
       </c>
@@ -4633,7 +4712,7 @@
         <v>554.14</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
         <v>25</v>
       </c>
@@ -4695,12 +4774,12 @@
         <v>-65.84</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>0</v>
       </c>
@@ -4747,7 +4826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -4786,7 +4865,7 @@
         <v>9.4973680564670149E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>0</v>
       </c>
@@ -4825,7 +4904,7 @@
         <v>5.7619441163551825E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>0</v>
       </c>
@@ -4864,7 +4943,7 @@
         <v>0.66229147661735754</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>0</v>
       </c>
@@ -4903,7 +4982,7 @@
         <v>0.43558007300610163</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>0</v>
       </c>
@@ -4942,9 +5021,254 @@
         <v>1.2614951446597022</v>
       </c>
     </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G44" t="s">
+        <v>39</v>
+      </c>
+      <c r="H44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I44" t="s">
+        <v>41</v>
+      </c>
+      <c r="J44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="16"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" t="s">
+        <v>31</v>
+      </c>
+      <c r="J46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2400</v>
+      </c>
+      <c r="B47">
+        <v>33</v>
+      </c>
+      <c r="C47">
+        <v>50</v>
+      </c>
+      <c r="D47">
+        <v>25</v>
+      </c>
+      <c r="E47">
+        <v>55</v>
+      </c>
+      <c r="F47">
+        <v>24</v>
+      </c>
+      <c r="G47">
+        <v>63</v>
+      </c>
+      <c r="H47">
+        <v>26.3</v>
+      </c>
+      <c r="J47">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2100</v>
+      </c>
+      <c r="B48">
+        <v>33</v>
+      </c>
+      <c r="C48">
+        <v>70</v>
+      </c>
+      <c r="D48">
+        <v>22</v>
+      </c>
+      <c r="E48">
+        <v>64</v>
+      </c>
+      <c r="F48">
+        <v>21</v>
+      </c>
+      <c r="G48">
+        <v>44</v>
+      </c>
+      <c r="H48">
+        <v>24.5</v>
+      </c>
+      <c r="J48">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1800</v>
+      </c>
+      <c r="B49">
+        <v>33</v>
+      </c>
+      <c r="C49">
+        <v>30</v>
+      </c>
+      <c r="D49">
+        <v>17</v>
+      </c>
+      <c r="E49">
+        <v>55</v>
+      </c>
+      <c r="F49">
+        <v>20</v>
+      </c>
+      <c r="G49">
+        <v>59</v>
+      </c>
+      <c r="H49">
+        <v>18</v>
+      </c>
+      <c r="J49">
+        <v>18.329999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1500</v>
+      </c>
+      <c r="B50">
+        <v>33</v>
+      </c>
+      <c r="C50">
+        <v>150</v>
+      </c>
+      <c r="D50">
+        <v>12</v>
+      </c>
+      <c r="E50">
+        <v>90</v>
+      </c>
+      <c r="F50">
+        <v>13</v>
+      </c>
+      <c r="G50">
+        <v>74</v>
+      </c>
+      <c r="H50">
+        <v>11</v>
+      </c>
+      <c r="J50">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1200</v>
+      </c>
+      <c r="B51">
+        <v>33</v>
+      </c>
+      <c r="C51">
+        <v>45</v>
+      </c>
+      <c r="D51">
+        <v>9</v>
+      </c>
+      <c r="E51">
+        <v>40</v>
+      </c>
+      <c r="F51">
+        <v>10</v>
+      </c>
+      <c r="G51">
+        <v>30</v>
+      </c>
+      <c r="H51">
+        <v>7</v>
+      </c>
+      <c r="J51">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>900</v>
+      </c>
+      <c r="B52">
+        <v>33</v>
+      </c>
+      <c r="C52">
+        <v>57</v>
+      </c>
+      <c r="D52">
+        <v>6</v>
+      </c>
+      <c r="E52">
+        <v>70</v>
+      </c>
+      <c r="F52">
+        <v>5</v>
+      </c>
+      <c r="G52">
+        <v>48</v>
+      </c>
+      <c r="H52">
+        <v>5</v>
+      </c>
+      <c r="J52">
+        <v>18.3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>